<commit_message>
add sort support for Product tree view. added more excel demo data for Product_Name
</commit_message>
<xml_diff>
--- a/addons/pharma-pos/demo_excel/pharma_pos.product_name.xlsx
+++ b/addons/pharma-pos/demo_excel/pharma_pos.product_name.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Generic Name</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>Losari</t>
+  </si>
+  <si>
+    <t>Ate</t>
+  </si>
+  <si>
+    <t>Atenolol</t>
+  </si>
+  <si>
+    <t>Colchi</t>
+  </si>
+  <si>
+    <t>Colchisin</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,6 +435,28 @@
         <v>44225</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>44227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <v>44227</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>